<commit_message>
Add testing accuracy for buble sheet
</commit_message>
<xml_diff>
--- a/src/bubble_sheet_results.xlsx
+++ b/src/bubble_sheet_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -67,7 +67,79 @@
     <t>Q16</t>
   </si>
   <si>
-    <t>0101</t>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>Q19</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q21</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>Q23</t>
+  </si>
+  <si>
+    <t>Q24</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>Q26</t>
+  </si>
+  <si>
+    <t>Q27</t>
+  </si>
+  <si>
+    <t>Q28</t>
+  </si>
+  <si>
+    <t>Q29</t>
+  </si>
+  <si>
+    <t>Q30</t>
+  </si>
+  <si>
+    <t>Q31</t>
+  </si>
+  <si>
+    <t>Q32</t>
+  </si>
+  <si>
+    <t>Q33</t>
+  </si>
+  <si>
+    <t>Q34</t>
+  </si>
+  <si>
+    <t>Q35</t>
+  </si>
+  <si>
+    <t>Q36</t>
+  </si>
+  <si>
+    <t>Q37</t>
+  </si>
+  <si>
+    <t>Q38</t>
+  </si>
+  <si>
+    <t>Q39</t>
+  </si>
+  <si>
+    <t>Q40</t>
+  </si>
+  <si>
+    <t>4521</t>
   </si>
 </sst>
 </file>
@@ -425,13 +497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:41">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,25 +555,97 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:41">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -516,24 +660,96 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
         <v>0</v>
       </c>
     </row>

</xml_diff>